<commit_message>
sat base model til SGD ingen momentum
</commit_message>
<xml_diff>
--- a/Results_CNN.xlsx
+++ b/Results_CNN.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S13"/>
+  <dimension ref="A1:T17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -529,6 +529,11 @@
           <t>Learning rate decay</t>
         </is>
       </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Gamma</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -596,6 +601,7 @@
       </c>
       <c r="R2" t="inlineStr"/>
       <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -663,6 +669,7 @@
       </c>
       <c r="R3" t="inlineStr"/>
       <c r="S3" t="inlineStr"/>
+      <c r="T3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -730,6 +737,7 @@
       </c>
       <c r="R4" t="inlineStr"/>
       <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -797,6 +805,7 @@
       </c>
       <c r="R5" t="inlineStr"/>
       <c r="S5" t="inlineStr"/>
+      <c r="T5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -864,6 +873,7 @@
       </c>
       <c r="R6" t="inlineStr"/>
       <c r="S6" t="inlineStr"/>
+      <c r="T6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -933,6 +943,7 @@
         <v>0</v>
       </c>
       <c r="S7" t="inlineStr"/>
+      <c r="T7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1002,6 +1013,7 @@
         <v>0.005</v>
       </c>
       <c r="S8" t="inlineStr"/>
+      <c r="T8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1071,6 +1083,7 @@
         <v>0.005</v>
       </c>
       <c r="S9" t="inlineStr"/>
+      <c r="T9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1140,6 +1153,7 @@
         <v>0.005</v>
       </c>
       <c r="S10" t="inlineStr"/>
+      <c r="T10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1209,6 +1223,7 @@
         <v>0.005</v>
       </c>
       <c r="S11" t="inlineStr"/>
+      <c r="T11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1278,6 +1293,7 @@
         <v>0.005</v>
       </c>
       <c r="S12" t="inlineStr"/>
+      <c r="T12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1351,6 +1367,293 @@
           <t>OneCycle</t>
         </is>
       </c>
+      <c r="T13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2024-1-4 21:19:16</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>20</v>
+      </c>
+      <c r="C14" t="n">
+        <v>64</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1.000000000000001e-12</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>SGD</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>35.9</v>
+      </c>
+      <c r="H14" t="n">
+        <v>32</v>
+      </c>
+      <c r="I14" t="n">
+        <v>1.7762</v>
+      </c>
+      <c r="J14" t="n">
+        <v>1.2311</v>
+      </c>
+      <c r="K14" t="n">
+        <v>45.3203</v>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+      <c r="N14" t="n">
+        <v>4</v>
+      </c>
+      <c r="O14" t="n">
+        <v>2</v>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q14" t="n">
+        <v>717.6847140835598</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0</v>
+      </c>
+      <c r="S14" t="inlineStr"/>
+      <c r="T14" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2024-1-4 22:27:24</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>20</v>
+      </c>
+      <c r="C15" t="n">
+        <v>64</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Adam</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>35.8</v>
+      </c>
+      <c r="H15" t="n">
+        <v>32</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.153</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.07099999999999999</v>
+      </c>
+      <c r="K15" t="n">
+        <v>97.405</v>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+      <c r="N15" t="n">
+        <v>4</v>
+      </c>
+      <c r="O15" t="n">
+        <v>2</v>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>Alfred</t>
+        </is>
+      </c>
+      <c r="Q15" t="n">
+        <v>716.4068887932226</v>
+      </c>
+      <c r="R15" t="n">
+        <v>0</v>
+      </c>
+      <c r="S15" t="inlineStr"/>
+      <c r="T15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2024-1-5 10:31:45</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>20</v>
+      </c>
+      <c r="C16" t="n">
+        <v>64</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Adam</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>37.2</v>
+      </c>
+      <c r="H16" t="n">
+        <v>32</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.214</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.1574</v>
+      </c>
+      <c r="K16" t="n">
+        <v>96.78149999999999</v>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+      <c r="N16" t="n">
+        <v>4</v>
+      </c>
+      <c r="O16" t="n">
+        <v>2</v>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>Alfred</t>
+        </is>
+      </c>
+      <c r="Q16" t="n">
+        <v>743.602515457198</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0</v>
+      </c>
+      <c r="S16" t="inlineStr"/>
+      <c r="T16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2024-1-5 10:45:27</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>20</v>
+      </c>
+      <c r="C17" t="n">
+        <v>64</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>SGD no momentum</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>35.9</v>
+      </c>
+      <c r="H17" t="n">
+        <v>32</v>
+      </c>
+      <c r="I17" t="n">
+        <v>1.3528</v>
+      </c>
+      <c r="J17" t="n">
+        <v>1.3307</v>
+      </c>
+      <c r="K17" t="n">
+        <v>51.4926</v>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+      <c r="N17" t="n">
+        <v>4</v>
+      </c>
+      <c r="O17" t="n">
+        <v>2</v>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>Alfred</t>
+        </is>
+      </c>
+      <c r="Q17" t="n">
+        <v>717.830478457734</v>
+      </c>
+      <c r="R17" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T17" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
ikke rigtig nogle ændringer
</commit_message>
<xml_diff>
--- a/Results_CNN.xlsx
+++ b/Results_CNN.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T17"/>
+  <dimension ref="A1:V18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -534,6 +534,16 @@
           <t>Gamma</t>
         </is>
       </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Scheduler</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Min. LR</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -602,6 +612,8 @@
       <c r="R2" t="inlineStr"/>
       <c r="S2" t="inlineStr"/>
       <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -670,6 +682,8 @@
       <c r="R3" t="inlineStr"/>
       <c r="S3" t="inlineStr"/>
       <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -738,6 +752,8 @@
       <c r="R4" t="inlineStr"/>
       <c r="S4" t="inlineStr"/>
       <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -806,6 +822,8 @@
       <c r="R5" t="inlineStr"/>
       <c r="S5" t="inlineStr"/>
       <c r="T5" t="inlineStr"/>
+      <c r="U5" t="inlineStr"/>
+      <c r="V5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -874,6 +892,8 @@
       <c r="R6" t="inlineStr"/>
       <c r="S6" t="inlineStr"/>
       <c r="T6" t="inlineStr"/>
+      <c r="U6" t="inlineStr"/>
+      <c r="V6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -944,6 +964,8 @@
       </c>
       <c r="S7" t="inlineStr"/>
       <c r="T7" t="inlineStr"/>
+      <c r="U7" t="inlineStr"/>
+      <c r="V7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1014,6 +1036,8 @@
       </c>
       <c r="S8" t="inlineStr"/>
       <c r="T8" t="inlineStr"/>
+      <c r="U8" t="inlineStr"/>
+      <c r="V8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1084,6 +1108,8 @@
       </c>
       <c r="S9" t="inlineStr"/>
       <c r="T9" t="inlineStr"/>
+      <c r="U9" t="inlineStr"/>
+      <c r="V9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1154,6 +1180,8 @@
       </c>
       <c r="S10" t="inlineStr"/>
       <c r="T10" t="inlineStr"/>
+      <c r="U10" t="inlineStr"/>
+      <c r="V10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1224,6 +1252,8 @@
       </c>
       <c r="S11" t="inlineStr"/>
       <c r="T11" t="inlineStr"/>
+      <c r="U11" t="inlineStr"/>
+      <c r="V11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1294,6 +1324,8 @@
       </c>
       <c r="S12" t="inlineStr"/>
       <c r="T12" t="inlineStr"/>
+      <c r="U12" t="inlineStr"/>
+      <c r="V12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1368,6 +1400,8 @@
         </is>
       </c>
       <c r="T13" t="inlineStr"/>
+      <c r="U13" t="inlineStr"/>
+      <c r="V13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1440,6 +1474,8 @@
       <c r="T14" t="n">
         <v>0.1</v>
       </c>
+      <c r="U14" t="inlineStr"/>
+      <c r="V14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1510,6 +1546,8 @@
       </c>
       <c r="S15" t="inlineStr"/>
       <c r="T15" t="inlineStr"/>
+      <c r="U15" t="inlineStr"/>
+      <c r="V15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1580,6 +1618,8 @@
       </c>
       <c r="S16" t="inlineStr"/>
       <c r="T16" t="inlineStr"/>
+      <c r="U16" t="inlineStr"/>
+      <c r="V16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1648,12 +1688,90 @@
       <c r="R17" t="n">
         <v>0.005</v>
       </c>
-      <c r="S17" t="inlineStr">
+      <c r="S17" t="inlineStr"/>
+      <c r="T17" t="inlineStr"/>
+      <c r="U17" t="inlineStr"/>
+      <c r="V17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2024-1-5 11:1:58</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>2</v>
+      </c>
+      <c r="C18" t="n">
+        <v>64</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>35.9</v>
+      </c>
+      <c r="H18" t="n">
+        <v>32</v>
+      </c>
+      <c r="I18" t="n">
+        <v>1.9151</v>
+      </c>
+      <c r="J18" t="n">
+        <v>1.7357</v>
+      </c>
+      <c r="K18" t="n">
+        <v>26.0162</v>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+      <c r="N18" t="n">
+        <v>4</v>
+      </c>
+      <c r="O18" t="n">
+        <v>2</v>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q18" t="n">
+        <v>71.7</v>
+      </c>
+      <c r="R18" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="S18" t="inlineStr"/>
+      <c r="T18" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="U18" t="inlineStr">
         <is>
           <t>None</t>
         </is>
       </c>
-      <c r="T17" t="inlineStr"/>
+      <c r="V18" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fixede accuracy til test data istedet for train data
</commit_message>
<xml_diff>
--- a/Results_CNN.xlsx
+++ b/Results_CNN.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -685,12 +685,162 @@
       <c r="S3" t="n">
         <v>0</v>
       </c>
-      <c r="T3" t="inlineStr">
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2024-1-6 14:16:55</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>10</v>
+      </c>
+      <c r="C4" t="n">
+        <v>64</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>36.4</v>
+      </c>
+      <c r="H4" t="n">
+        <v>32</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.6728</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.5442</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.5196433546949011</v>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+      <c r="N4" t="n">
+        <v>4</v>
+      </c>
+      <c r="O4" t="n">
+        <v>2</v>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>Alfred</t>
+        </is>
+      </c>
+      <c r="Q4" t="n">
+        <v>364.4</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2024-1-6 14:32:46</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>10</v>
+      </c>
+      <c r="C5" t="n">
+        <v>64</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>ADAM</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>36.9</v>
+      </c>
+      <c r="H5" t="n">
+        <v>32</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1.0813</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1.0813</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.515881861242686</v>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+      <c r="N5" t="n">
+        <v>4</v>
+      </c>
+      <c r="O5" t="n">
+        <v>2</v>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Alfred</t>
+        </is>
+      </c>
+      <c r="Q5" t="n">
+        <v>369.3</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="T5" t="inlineStr">
         <is>
           <t>None</t>
         </is>
       </c>
-      <c r="U3" t="n">
+      <c r="U5" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
flere forskellige models,  tilføjede data augmentation
</commit_message>
<xml_diff>
--- a/Results_CNN.xlsx
+++ b/Results_CNN.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U5"/>
+  <dimension ref="A1:U18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -835,12 +835,959 @@
       <c r="S5" t="n">
         <v>0.005</v>
       </c>
-      <c r="T5" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="T5" t="inlineStr"/>
       <c r="U5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2024-1-6 18:15:25</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>40</v>
+      </c>
+      <c r="C6" t="n">
+        <v>64</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>36.5</v>
+      </c>
+      <c r="H6" t="n">
+        <v>32</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.2338</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.0268</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.523822791864029</v>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+      <c r="N6" t="n">
+        <v>4</v>
+      </c>
+      <c r="O6" t="n">
+        <v>2</v>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q6" t="n">
+        <v>1459.7</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="T6" t="inlineStr"/>
+      <c r="U6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2024-1-6 18:52:52</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>40</v>
+      </c>
+      <c r="C7" t="n">
+        <v>128</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>34.6</v>
+      </c>
+      <c r="H7" t="n">
+        <v>32</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.0273</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.0273</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.5200612984118139</v>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+      <c r="N7" t="n">
+        <v>4</v>
+      </c>
+      <c r="O7" t="n">
+        <v>2</v>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>Stationær</t>
+        </is>
+      </c>
+      <c r="Q7" t="n">
+        <v>1382.9</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="T7" t="inlineStr"/>
+      <c r="U7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2024-1-6 19:25:59</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>40</v>
+      </c>
+      <c r="C8" t="n">
+        <v>64</v>
+      </c>
+      <c r="D8" t="n">
+        <v>4.8828125e-06</v>
+      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>38.4</v>
+      </c>
+      <c r="H8" t="n">
+        <v>32</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.6402</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.4959</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.4891334633602675</v>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+      <c r="N8" t="n">
+        <v>4</v>
+      </c>
+      <c r="O8" t="n">
+        <v>2</v>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>Alfred</t>
+        </is>
+      </c>
+      <c r="Q8" t="n">
+        <v>1537.8</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>AliLR</t>
+        </is>
+      </c>
+      <c r="U8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2024-1-6 19:45:57</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>40</v>
+      </c>
+      <c r="C9" t="n">
+        <v>64</v>
+      </c>
+      <c r="D9" t="n">
+        <v>4.8828125e-06</v>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>13</v>
+      </c>
+      <c r="H9" t="n">
+        <v>32</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1.4975</v>
+      </c>
+      <c r="J9" t="n">
+        <v>1.1526</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.4395374756199498</v>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+      <c r="N9" t="n">
+        <v>4</v>
+      </c>
+      <c r="O9" t="n">
+        <v>2</v>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>Alfred</t>
+        </is>
+      </c>
+      <c r="Q9" t="n">
+        <v>519.9</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>AliLR</t>
+        </is>
+      </c>
+      <c r="U9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2024-1-6 19:58:41</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>40</v>
+      </c>
+      <c r="C10" t="n">
+        <v>64</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>13.4</v>
+      </c>
+      <c r="H10" t="n">
+        <v>32</v>
+      </c>
+      <c r="I10" t="n">
+        <v>1.5033</v>
+      </c>
+      <c r="J10" t="n">
+        <v>1.2133</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.4460852605182502</v>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+      <c r="N10" t="n">
+        <v>4</v>
+      </c>
+      <c r="O10" t="n">
+        <v>2</v>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>Alfred</t>
+        </is>
+      </c>
+      <c r="Q10" t="n">
+        <v>536.5</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="T10" t="inlineStr"/>
+      <c r="U10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2024-1-6 20:10:6</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>40</v>
+      </c>
+      <c r="C11" t="n">
+        <v>64</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>12.6</v>
+      </c>
+      <c r="H11" t="n">
+        <v>32</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.8162</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.5788</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.4545834494288102</v>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+      <c r="N11" t="n">
+        <v>4</v>
+      </c>
+      <c r="O11" t="n">
+        <v>2</v>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>Alfred</t>
+        </is>
+      </c>
+      <c r="Q11" t="n">
+        <v>502.3</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0</v>
+      </c>
+      <c r="T11" t="inlineStr"/>
+      <c r="U11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2024-1-6 20:20:21</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>40</v>
+      </c>
+      <c r="C12" t="n">
+        <v>64</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>12.8</v>
+      </c>
+      <c r="H12" t="n">
+        <v>32</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.8093</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.6456</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.4660072443577598</v>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+      <c r="N12" t="n">
+        <v>4</v>
+      </c>
+      <c r="O12" t="n">
+        <v>2</v>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>Alfred</t>
+        </is>
+      </c>
+      <c r="Q12" t="n">
+        <v>511.4</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0</v>
+      </c>
+      <c r="S12" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="T12" t="inlineStr"/>
+      <c r="U12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2024-1-6 20:32:37</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>40</v>
+      </c>
+      <c r="C13" t="n">
+        <v>128</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>12.8</v>
+      </c>
+      <c r="H13" t="n">
+        <v>32</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.8465</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.7662</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.4534689328503761</v>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+      <c r="N13" t="n">
+        <v>4</v>
+      </c>
+      <c r="O13" t="n">
+        <v>2</v>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>Alfred</t>
+        </is>
+      </c>
+      <c r="Q13" t="n">
+        <v>511.2</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0</v>
+      </c>
+      <c r="S13" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="T13" t="inlineStr"/>
+      <c r="U13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2024-1-6 20:43:14</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>40</v>
+      </c>
+      <c r="C14" t="n">
+        <v>128</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>12.6</v>
+      </c>
+      <c r="H14" t="n">
+        <v>32</v>
+      </c>
+      <c r="I14" t="n">
+        <v>1.0993</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.829</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.4668431317915854</v>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+      <c r="N14" t="n">
+        <v>4</v>
+      </c>
+      <c r="O14" t="n">
+        <v>2</v>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>Alfred</t>
+        </is>
+      </c>
+      <c r="Q14" t="n">
+        <v>503</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S14" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="T14" t="inlineStr">
+        <is>
+          <t>OneCircleLR</t>
+        </is>
+      </c>
+      <c r="U14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2024-1-6 21:15:16</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>100</v>
+      </c>
+      <c r="C15" t="n">
+        <v>64</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="H15" t="n">
+        <v>32</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.6294999999999999</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.5351</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.4584842574533296</v>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+      <c r="N15" t="n">
+        <v>4</v>
+      </c>
+      <c r="O15" t="n">
+        <v>2</v>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>Alfred</t>
+        </is>
+      </c>
+      <c r="Q15" t="n">
+        <v>1325.9</v>
+      </c>
+      <c r="R15" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S15" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>CosineAnnealingLR</t>
+        </is>
+      </c>
+      <c r="U15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2024-1-6 22:26:7</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>100</v>
+      </c>
+      <c r="C16" t="n">
+        <v>64</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>37.2</v>
+      </c>
+      <c r="H16" t="n">
+        <v>32</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.0581</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.0133</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0.5118417386458624</v>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+      <c r="N16" t="n">
+        <v>4</v>
+      </c>
+      <c r="O16" t="n">
+        <v>2</v>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>Alfred</t>
+        </is>
+      </c>
+      <c r="Q16" t="n">
+        <v>3720.5</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S16" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>CosineAnnealingLR</t>
+        </is>
+      </c>
+      <c r="U16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2024-1-6 23:20:15</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>100</v>
+      </c>
+      <c r="C17" t="n">
+        <v>64</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.0008950775061868627</v>
+      </c>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>39.7</v>
+      </c>
+      <c r="H17" t="n">
+        <v>32</v>
+      </c>
+      <c r="I17" t="n">
+        <v>1.1311</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.7085</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.5628308721092227</v>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+      <c r="N17" t="n">
+        <v>4</v>
+      </c>
+      <c r="O17" t="n">
+        <v>2</v>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>Alfred</t>
+        </is>
+      </c>
+      <c r="Q17" t="n">
+        <v>1191.3</v>
+      </c>
+      <c r="R17" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S17" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t>CosineAnnealingLR</t>
+        </is>
+      </c>
+      <c r="U17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2024-1-7 1:35:49</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>100</v>
+      </c>
+      <c r="C18" t="n">
+        <v>64</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>70.09999999999999</v>
+      </c>
+      <c r="H18" t="n">
+        <v>32</v>
+      </c>
+      <c r="I18" t="n">
+        <v>1.0657</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.722</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.5824742268041238</v>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+      <c r="N18" t="n">
+        <v>4</v>
+      </c>
+      <c r="O18" t="n">
+        <v>2</v>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>Alfred</t>
+        </is>
+      </c>
+      <c r="Q18" t="n">
+        <v>7011.5</v>
+      </c>
+      <c r="R18" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S18" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="T18" t="inlineStr">
+        <is>
+          <t>CosineAnnealingLR</t>
+        </is>
+      </c>
+      <c r="U18" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Tilføjet batch normilization, early stoppage, 48x48 pixels, forskellige models, data augemnetation
</commit_message>
<xml_diff>
--- a/Results_CNN.xlsx
+++ b/Results_CNN.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U18"/>
+  <dimension ref="A1:U25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1791,6 +1791,527 @@
         <v>0</v>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2024-1-7 10:27:59</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>40</v>
+      </c>
+      <c r="C19" t="n">
+        <v>32</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
+        <v>73.40000000000001</v>
+      </c>
+      <c r="H19" t="n">
+        <v>32</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.8885</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0.5395653385344107</v>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+      <c r="N19" t="n">
+        <v>4</v>
+      </c>
+      <c r="O19" t="n">
+        <v>2</v>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>Alfred</t>
+        </is>
+      </c>
+      <c r="Q19" t="n">
+        <v>2935.5</v>
+      </c>
+      <c r="R19" t="n">
+        <v>0</v>
+      </c>
+      <c r="S19" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="T19" t="inlineStr"/>
+      <c r="U19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2024-1-7 11:29:54</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>40</v>
+      </c>
+      <c r="C20" t="n">
+        <v>64</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>68.59999999999999</v>
+      </c>
+      <c r="H20" t="n">
+        <v>32</v>
+      </c>
+      <c r="I20" t="n">
+        <v>1.5505</v>
+      </c>
+      <c r="J20" t="n">
+        <v>1.4351</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0.4086096405684034</v>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+      <c r="N20" t="n">
+        <v>4</v>
+      </c>
+      <c r="O20" t="n">
+        <v>2</v>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>Alfred</t>
+        </is>
+      </c>
+      <c r="Q20" t="n">
+        <v>2745.2</v>
+      </c>
+      <c r="R20" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S20" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="T20" t="inlineStr">
+        <is>
+          <t>ExponentialLR</t>
+        </is>
+      </c>
+      <c r="U20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2024-1-7 13:5:31</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>40</v>
+      </c>
+      <c r="C21" t="n">
+        <v>64</v>
+      </c>
+      <c r="D21" t="n">
+        <v>4.8828125e-05</v>
+      </c>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G21" t="n">
+        <v>15.8</v>
+      </c>
+      <c r="H21" t="n">
+        <v>32</v>
+      </c>
+      <c r="I21" t="n">
+        <v>1.3176</v>
+      </c>
+      <c r="J21" t="n">
+        <v>1.1116</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0.4967957648370019</v>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+      <c r="N21" t="n">
+        <v>4</v>
+      </c>
+      <c r="O21" t="n">
+        <v>2</v>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>Alfred</t>
+        </is>
+      </c>
+      <c r="Q21" t="n">
+        <v>633.5</v>
+      </c>
+      <c r="R21" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S21" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="T21" t="inlineStr">
+        <is>
+          <t>AliLR</t>
+        </is>
+      </c>
+      <c r="U21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2024-1-7 13:29:50</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>100</v>
+      </c>
+      <c r="C22" t="n">
+        <v>64</v>
+      </c>
+      <c r="D22" t="n">
+        <v>3.90625e-05</v>
+      </c>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
+        <v>15.7</v>
+      </c>
+      <c r="H22" t="n">
+        <v>32</v>
+      </c>
+      <c r="I22" t="n">
+        <v>1.2793</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0.9649</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0.5275842853162441</v>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+      <c r="N22" t="n">
+        <v>4</v>
+      </c>
+      <c r="O22" t="n">
+        <v>2</v>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>Alfred</t>
+        </is>
+      </c>
+      <c r="Q22" t="n">
+        <v>1272.3</v>
+      </c>
+      <c r="R22" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S22" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="T22" t="inlineStr">
+        <is>
+          <t>AliLR</t>
+        </is>
+      </c>
+      <c r="U22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2024-1-7 15:9:56</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>100</v>
+      </c>
+      <c r="C23" t="n">
+        <v>64</v>
+      </c>
+      <c r="D23" t="n">
+        <v>9.765625e-06</v>
+      </c>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G23" t="n">
+        <v>22.8</v>
+      </c>
+      <c r="H23" t="n">
+        <v>32</v>
+      </c>
+      <c r="I23" t="n">
+        <v>1.427</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0.784</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0.5125383115073837</v>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+      <c r="N23" t="n">
+        <v>4</v>
+      </c>
+      <c r="O23" t="n">
+        <v>2</v>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>Alfred</t>
+        </is>
+      </c>
+      <c r="Q23" t="n">
+        <v>2282.2</v>
+      </c>
+      <c r="R23" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S23" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="T23" t="inlineStr">
+        <is>
+          <t>AliLR</t>
+        </is>
+      </c>
+      <c r="U23" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2024-1-7 15:39:12</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>30</v>
+      </c>
+      <c r="C24" t="n">
+        <v>64</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.00015625</v>
+      </c>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G24" t="n">
+        <v>67.40000000000001</v>
+      </c>
+      <c r="H24" t="n">
+        <v>32</v>
+      </c>
+      <c r="I24" t="n">
+        <v>1.7425</v>
+      </c>
+      <c r="J24" t="n">
+        <v>1.3977</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0.3507940930621343</v>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+      <c r="N24" t="n">
+        <v>4</v>
+      </c>
+      <c r="O24" t="n">
+        <v>2</v>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>Alfred</t>
+        </is>
+      </c>
+      <c r="Q24" t="n">
+        <v>1281.5</v>
+      </c>
+      <c r="R24" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S24" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="T24" t="inlineStr">
+        <is>
+          <t>AliLR</t>
+        </is>
+      </c>
+      <c r="U24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2024-1-7 18:12:38</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>100</v>
+      </c>
+      <c r="C25" t="n">
+        <v>64</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>CEL</t>
+        </is>
+      </c>
+      <c r="G25" t="n">
+        <v>68.5</v>
+      </c>
+      <c r="H25" t="n">
+        <v>32</v>
+      </c>
+      <c r="I25" t="n">
+        <v>1.1024</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0.5744</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0.6058790749512399</v>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>FER2013</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+      <c r="N25" t="n">
+        <v>4</v>
+      </c>
+      <c r="O25" t="n">
+        <v>2</v>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>Alfred</t>
+        </is>
+      </c>
+      <c r="Q25" t="n">
+        <v>5340.4</v>
+      </c>
+      <c r="R25" t="n">
+        <v>0</v>
+      </c>
+      <c r="S25" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="T25" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="U25" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>